<commit_message>
updated scope and windows documentation
</commit_message>
<xml_diff>
--- a/reference/docs/SAMBUCA Scope.xlsx
+++ b/reference/docs/SAMBUCA Scope.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\sambuca\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\sambuca\reference\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1090,7 +1090,7 @@
   <dimension ref="A1:G151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,7 +1138,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>33</v>
@@ -1155,7 +1155,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1169,7 +1169,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1183,7 +1183,7 @@
         <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>25</v>
@@ -1254,7 +1254,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>15</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>42</v>
@@ -1316,7 +1316,7 @@
         <v>9</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>29</v>

</xml_diff>